<commit_message>
Added extract games from web
</commit_message>
<xml_diff>
--- a/SteamLibrary/GamesToAdd.xlsx
+++ b/SteamLibrary/GamesToAdd.xlsx
@@ -22,52 +22,52 @@
     <x:t>Status</x:t>
   </x:si>
   <x:si>
-    <x:t>Children of Silentown: Prologue</x:t>
+    <x:t>Nomads of Driftland</x:t>
   </x:si>
   <x:si>
     <x:t>Added</x:t>
   </x:si>
   <x:si>
-    <x:t>Is It Wrong to Try to Shoot 'em Up Girls in a Dungeon?</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Floor Is Still Really Cheap Lava</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ball at Work: A Fun and Unique Game of Skill and Patience!</x:t>
-  </x:si>
-  <x:si>
-    <x:t>VR Only Eggs Catcher VR</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SUPERCHICOS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Toast Defense</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tiny Toy Tanks</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BatuGame</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Phobos</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Aurora: A Child's Journey</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Tenami</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Verse Surf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Super Buckyball Tournament Preseason</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Daikaiju Daikessen: Versus</x:t>
+    <x:t>Slapshot: Rebound</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Leaf Blower Revolution - Idle Game</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Summerland</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ruff Night At The Gallery</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rubber Bandits: Christmas Prologue</x:t>
+  </x:si>
+  <x:si>
+    <x:t>The Life and Suffering of Sir Brante — Chapter 1&amp;2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AOD: Art Of Defense</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mrs. Santa's Gift Hunt</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ninja Hanrei</x:t>
+  </x:si>
+  <x:si>
+    <x:t>*NEW* SCUFFED EPIC BHOP SIMULATOR 2023 (POG CHAMP)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DreamWatcher</x:t>
+  </x:si>
+  <x:si>
+    <x:t>From the Shadows</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KAKU: Ancient Seal (Alpha)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Night Reverie: Prologue</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>